<commit_message>
ckt updated with hazard detection skeleton
</commit_message>
<xml_diff>
--- a/Project 1/Report/Project1Data.xlsx
+++ b/Project 1/Report/Project1Data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sleon\Documents\Git\computer-architecture\Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdjoh\Documents\GitHub\computer-architecture\Project 1\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1200" windowWidth="17250" windowHeight="5670"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="17250" windowHeight="5670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="115">
   <si>
     <t>Input(s)</t>
   </si>
@@ -253,6 +254,123 @@
   </si>
   <si>
     <t>Timer_Overwrite</t>
+  </si>
+  <si>
+    <t>IF/ID Register</t>
+  </si>
+  <si>
+    <t>Instruction_IN</t>
+  </si>
+  <si>
+    <t>PC_IN</t>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t>Instruction_OUT</t>
+  </si>
+  <si>
+    <t>PC_OUT</t>
+  </si>
+  <si>
+    <t>ID/EX Register</t>
+  </si>
+  <si>
+    <t>WB_IN</t>
+  </si>
+  <si>
+    <t>M_IN</t>
+  </si>
+  <si>
+    <t>EX_IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC_IN </t>
+  </si>
+  <si>
+    <t>Read_Data1_IN</t>
+  </si>
+  <si>
+    <t>Read_Data2_IN</t>
+  </si>
+  <si>
+    <t>Extended_Data_IN</t>
+  </si>
+  <si>
+    <t>Temp1_IN</t>
+  </si>
+  <si>
+    <t>RD_IN</t>
+  </si>
+  <si>
+    <t>WB_OUT</t>
+  </si>
+  <si>
+    <t>M_OUT</t>
+  </si>
+  <si>
+    <t>EX_OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PC_OUT </t>
+  </si>
+  <si>
+    <t>Read_Data1_OUT</t>
+  </si>
+  <si>
+    <t>Read_Data2_OUT</t>
+  </si>
+  <si>
+    <t>Extended_Data_OUT</t>
+  </si>
+  <si>
+    <t>Temp1_OUT</t>
+  </si>
+  <si>
+    <t>RD_OUT</t>
+  </si>
+  <si>
+    <t>EX/MEM Register</t>
+  </si>
+  <si>
+    <t>Zero_IN</t>
+  </si>
+  <si>
+    <t>Negative_IN</t>
+  </si>
+  <si>
+    <t>ALU_Res_IN</t>
+  </si>
+  <si>
+    <t>ReadData2_IN</t>
+  </si>
+  <si>
+    <t>Zero_OUT</t>
+  </si>
+  <si>
+    <t>Negative_OUT</t>
+  </si>
+  <si>
+    <t>ALU_Res_OUT</t>
+  </si>
+  <si>
+    <t>ReadData2_OUT</t>
+  </si>
+  <si>
+    <t>MEM/WB Register</t>
+  </si>
+  <si>
+    <t>ReadData_IN</t>
+  </si>
+  <si>
+    <t>Rd_IN</t>
+  </si>
+  <si>
+    <t>ReadData_OUT</t>
+  </si>
+  <si>
+    <t>Rd_OUT</t>
   </si>
 </sst>
 </file>
@@ -687,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,10 +1526,361 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="D1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="11"/>
+      <c r="G1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="11"/>
+      <c r="J1" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="K1" s="11"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="D5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="D6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="10"/>
+      <c r="D7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="10"/>
+      <c r="D8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="10"/>
+      <c r="D9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="10"/>
+      <c r="D10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="10"/>
+      <c r="D11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="10"/>
+      <c r="D12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="G12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="10"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="10"/>
+      <c r="D13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="10"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="10"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="10"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="10"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="10"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="10"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="10"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="10"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="10"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="10"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="10"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="10"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="10"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="10"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="10"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="10"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="10"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>